<commit_message>
updated pcb stackup and silkscreen top
</commit_message>
<xml_diff>
--- a/P60/rev5/p60-dock/PCB_order.xlsx
+++ b/P60/rev5/p60-dock/PCB_order.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr codeName="Denne_projektmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bgs\dev\Hardware\nanopower\P60\rev5\p60-dock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3452E6B1-54D8-4608-8F21-F803AD73C210}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E9A6356-1FE3-4274-BCDD-A723A4F6608E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9510" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PCB Specifications" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,19 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'PCB Specifications'!$B$2:$H$59</definedName>
     <definedName name="R_">'PCB Specifications'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="145">
   <si>
     <t>Read-Me File</t>
   </si>
@@ -365,9 +372,6 @@
   </si>
   <si>
     <t>Brian Gasberg Thomsen</t>
-  </si>
-  <si>
-    <t>4.0</t>
   </si>
   <si>
     <t>GND plane</t>
@@ -1370,111 +1374,147 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="1" fontId="0" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="15" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
@@ -1512,140 +1552,104 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="15" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -4825,8 +4829,8 @@
   </sheetPr>
   <dimension ref="A1:O337"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4845,222 +4849,222 @@
   <sheetData>
     <row r="1" spans="2:8" s="14" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="101" t="s">
+      <c r="B2" s="144" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="102"/>
-      <c r="D2" s="103"/>
+      <c r="C2" s="145"/>
+      <c r="D2" s="146"/>
       <c r="E2" s="31"/>
       <c r="F2" s="30"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="97"/>
+      <c r="G2" s="141"/>
+      <c r="H2" s="142"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="147" t="s">
         <v>106</v>
       </c>
-      <c r="C3" s="105"/>
-      <c r="D3" s="106"/>
+      <c r="C3" s="148"/>
+      <c r="D3" s="149"/>
       <c r="E3" s="32"/>
       <c r="F3" s="27"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="99"/>
+      <c r="G3" s="129"/>
+      <c r="H3" s="143"/>
     </row>
     <row r="4" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="107" t="s">
+      <c r="B4" s="150" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="108"/>
-      <c r="D4" s="109"/>
+      <c r="C4" s="151"/>
+      <c r="D4" s="152"/>
       <c r="E4" s="32"/>
       <c r="F4" s="27"/>
-      <c r="G4" s="98"/>
-      <c r="H4" s="99"/>
+      <c r="G4" s="129"/>
+      <c r="H4" s="143"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="107" t="s">
+      <c r="B5" s="150" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="108"/>
-      <c r="D5" s="109"/>
+      <c r="C5" s="151"/>
+      <c r="D5" s="152"/>
       <c r="E5" s="32"/>
       <c r="F5" s="27"/>
-      <c r="G5" s="98"/>
-      <c r="H5" s="99"/>
+      <c r="G5" s="129"/>
+      <c r="H5" s="143"/>
     </row>
     <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="110" t="s">
+      <c r="B6" s="153" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="111"/>
-      <c r="D6" s="112"/>
+      <c r="C6" s="154"/>
+      <c r="D6" s="155"/>
       <c r="E6" s="33"/>
       <c r="F6" s="34"/>
       <c r="G6" s="34"/>
       <c r="H6" s="35"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="113"/>
-      <c r="C7" s="114"/>
-      <c r="D7" s="114"/>
-      <c r="E7" s="114"/>
-      <c r="F7" s="114"/>
-      <c r="G7" s="114"/>
-      <c r="H7" s="115"/>
+      <c r="B7" s="156"/>
+      <c r="C7" s="157"/>
+      <c r="D7" s="157"/>
+      <c r="E7" s="157"/>
+      <c r="F7" s="157"/>
+      <c r="G7" s="157"/>
+      <c r="H7" s="158"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="95"/>
-      <c r="C8" s="118" t="s">
+      <c r="B8" s="161"/>
+      <c r="C8" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="156"/>
-      <c r="E8" s="156"/>
-      <c r="F8" s="157"/>
-      <c r="G8" s="153">
+      <c r="D8" s="87"/>
+      <c r="E8" s="87"/>
+      <c r="F8" s="88"/>
+      <c r="G8" s="92">
         <f ca="1">TODAY()</f>
-        <v>43250</v>
-      </c>
-      <c r="H8" s="91"/>
+        <v>43342</v>
+      </c>
+      <c r="H8" s="93"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="95"/>
-      <c r="C9" s="158" t="s">
+      <c r="B9" s="161"/>
+      <c r="C9" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="159"/>
-      <c r="E9" s="159"/>
-      <c r="F9" s="160"/>
-      <c r="G9" s="154" t="s">
+      <c r="D9" s="90"/>
+      <c r="E9" s="90"/>
+      <c r="F9" s="91"/>
+      <c r="G9" s="94" t="s">
         <v>107</v>
       </c>
-      <c r="H9" s="155"/>
+      <c r="H9" s="95"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="95"/>
-      <c r="C10" s="118" t="s">
+      <c r="B10" s="161"/>
+      <c r="C10" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="156"/>
-      <c r="E10" s="156"/>
-      <c r="F10" s="157"/>
-      <c r="G10" s="86">
-        <v>5881</v>
-      </c>
-      <c r="H10" s="91"/>
+      <c r="D10" s="87"/>
+      <c r="E10" s="87"/>
+      <c r="F10" s="88"/>
+      <c r="G10" s="96">
+        <v>105881</v>
+      </c>
+      <c r="H10" s="93"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="95"/>
-      <c r="C11" s="158" t="s">
+      <c r="B11" s="161"/>
+      <c r="C11" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="159"/>
-      <c r="E11" s="159"/>
-      <c r="F11" s="160"/>
-      <c r="G11" s="154" t="s">
-        <v>109</v>
-      </c>
-      <c r="H11" s="155"/>
+      <c r="D11" s="90"/>
+      <c r="E11" s="90"/>
+      <c r="F11" s="91"/>
+      <c r="G11" s="94">
+        <v>5</v>
+      </c>
+      <c r="H11" s="95"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="95"/>
-      <c r="C12" s="118" t="s">
+      <c r="B12" s="161"/>
+      <c r="C12" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="156"/>
-      <c r="E12" s="156"/>
-      <c r="F12" s="157"/>
-      <c r="G12" s="86" t="s">
+      <c r="D12" s="87"/>
+      <c r="E12" s="87"/>
+      <c r="F12" s="88"/>
+      <c r="G12" s="96" t="s">
         <v>108</v>
       </c>
-      <c r="H12" s="91"/>
+      <c r="H12" s="93"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="95"/>
-      <c r="C13" s="88" t="s">
+      <c r="B13" s="161"/>
+      <c r="C13" s="159" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="88"/>
-      <c r="E13" s="88"/>
-      <c r="F13" s="88"/>
-      <c r="G13" s="88"/>
-      <c r="H13" s="89"/>
+      <c r="D13" s="159"/>
+      <c r="E13" s="159"/>
+      <c r="F13" s="159"/>
+      <c r="G13" s="159"/>
+      <c r="H13" s="160"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="95"/>
-      <c r="C14" s="86" t="s">
+      <c r="B14" s="161"/>
+      <c r="C14" s="96" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="86" t="s">
+      <c r="D14" s="96"/>
+      <c r="E14" s="96"/>
+      <c r="F14" s="96"/>
+      <c r="G14" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="H14" s="91"/>
+      <c r="H14" s="93"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="95"/>
-      <c r="C15" s="87" t="s">
+      <c r="B15" s="161"/>
+      <c r="C15" s="99" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="87"/>
-      <c r="E15" s="87"/>
-      <c r="F15" s="87"/>
-      <c r="G15" s="87" t="s">
+      <c r="D15" s="99"/>
+      <c r="E15" s="99"/>
+      <c r="F15" s="99"/>
+      <c r="G15" s="99" t="s">
         <v>52</v>
       </c>
-      <c r="H15" s="90"/>
+      <c r="H15" s="100"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="95"/>
-      <c r="C16" s="86" t="s">
+      <c r="B16" s="161"/>
+      <c r="C16" s="96" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="86"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="86"/>
-      <c r="G16" s="86" t="s">
+      <c r="D16" s="96"/>
+      <c r="E16" s="96"/>
+      <c r="F16" s="96"/>
+      <c r="G16" s="96" t="s">
         <v>53</v>
       </c>
-      <c r="H16" s="91"/>
+      <c r="H16" s="93"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="95"/>
-      <c r="C17" s="87" t="s">
+      <c r="B17" s="161"/>
+      <c r="C17" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="87"/>
-      <c r="E17" s="87"/>
-      <c r="F17" s="87"/>
-      <c r="G17" s="87">
+      <c r="D17" s="99"/>
+      <c r="E17" s="99"/>
+      <c r="F17" s="99"/>
+      <c r="G17" s="99">
         <v>12</v>
       </c>
-      <c r="H17" s="90"/>
+      <c r="H17" s="100"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="95"/>
-      <c r="C18" s="86" t="s">
+      <c r="B18" s="161"/>
+      <c r="C18" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="86"/>
-      <c r="E18" s="86"/>
-      <c r="F18" s="86"/>
-      <c r="G18" s="151" t="s">
+      <c r="D18" s="96"/>
+      <c r="E18" s="96"/>
+      <c r="F18" s="96"/>
+      <c r="G18" s="97" t="s">
         <v>94</v>
       </c>
-      <c r="H18" s="152"/>
+      <c r="H18" s="98"/>
     </row>
     <row r="19" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="25"/>
-      <c r="B19" s="92" t="s">
+      <c r="B19" s="115" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="93"/>
-      <c r="D19" s="93"/>
-      <c r="E19" s="93"/>
-      <c r="F19" s="93"/>
-      <c r="G19" s="93"/>
-      <c r="H19" s="94"/>
+      <c r="C19" s="116"/>
+      <c r="D19" s="116"/>
+      <c r="E19" s="116"/>
+      <c r="F19" s="116"/>
+      <c r="G19" s="116"/>
+      <c r="H19" s="117"/>
       <c r="I19" s="25"/>
       <c r="J19" s="25"/>
       <c r="K19" s="25"/>
@@ -5072,16 +5076,16 @@
     <row r="20" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="25"/>
       <c r="B20" s="2"/>
-      <c r="C20" s="86" t="s">
+      <c r="C20" s="96" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="86"/>
-      <c r="E20" s="86"/>
-      <c r="F20" s="86"/>
-      <c r="G20" s="86" t="s">
+      <c r="D20" s="96"/>
+      <c r="E20" s="96"/>
+      <c r="F20" s="96"/>
+      <c r="G20" s="96" t="s">
         <v>48</v>
       </c>
-      <c r="H20" s="91"/>
+      <c r="H20" s="93"/>
       <c r="I20" s="25"/>
       <c r="J20" s="25"/>
       <c r="K20" s="25"/>
@@ -5093,16 +5097,16 @@
     <row r="21" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="87" t="s">
+      <c r="C21" s="99" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="87"/>
-      <c r="E21" s="87"/>
-      <c r="F21" s="87"/>
-      <c r="G21" s="87" t="s">
+      <c r="D21" s="99"/>
+      <c r="E21" s="99"/>
+      <c r="F21" s="99"/>
+      <c r="G21" s="99" t="s">
         <v>48</v>
       </c>
-      <c r="H21" s="90"/>
+      <c r="H21" s="100"/>
       <c r="I21" s="25"/>
       <c r="J21" s="25"/>
       <c r="K21" s="25"/>
@@ -5114,16 +5118,16 @@
     <row r="22" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="25"/>
       <c r="B22" s="2"/>
-      <c r="C22" s="86" t="s">
+      <c r="C22" s="96" t="s">
         <v>103</v>
       </c>
-      <c r="D22" s="86"/>
-      <c r="E22" s="86"/>
-      <c r="F22" s="86"/>
-      <c r="G22" s="86" t="s">
+      <c r="D22" s="96"/>
+      <c r="E22" s="96"/>
+      <c r="F22" s="96"/>
+      <c r="G22" s="96" t="s">
         <v>100</v>
       </c>
-      <c r="H22" s="91"/>
+      <c r="H22" s="93"/>
       <c r="I22" s="25"/>
       <c r="J22" s="25"/>
       <c r="K22" s="25"/>
@@ -5135,16 +5139,16 @@
     <row r="23" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="25"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="87" t="s">
+      <c r="C23" s="99" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="87"/>
-      <c r="E23" s="87"/>
-      <c r="F23" s="87"/>
-      <c r="G23" s="87" t="s">
+      <c r="D23" s="99"/>
+      <c r="E23" s="99"/>
+      <c r="F23" s="99"/>
+      <c r="G23" s="99" t="s">
         <v>57</v>
       </c>
-      <c r="H23" s="90"/>
+      <c r="H23" s="100"/>
       <c r="I23" s="25"/>
       <c r="J23" s="25"/>
       <c r="K23" s="25"/>
@@ -5156,16 +5160,16 @@
     <row r="24" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="25"/>
       <c r="B24" s="2"/>
-      <c r="C24" s="86" t="s">
+      <c r="C24" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="D24" s="86"/>
-      <c r="E24" s="86"/>
-      <c r="F24" s="86"/>
-      <c r="G24" s="86" t="s">
+      <c r="D24" s="96"/>
+      <c r="E24" s="96"/>
+      <c r="F24" s="96"/>
+      <c r="G24" s="96" t="s">
         <v>101</v>
       </c>
-      <c r="H24" s="91"/>
+      <c r="H24" s="93"/>
       <c r="I24" s="25"/>
       <c r="J24" s="25"/>
       <c r="K24" s="25"/>
@@ -5177,16 +5181,16 @@
     <row r="25" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="25"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="87" t="s">
+      <c r="C25" s="99" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="87"/>
-      <c r="E25" s="87"/>
-      <c r="F25" s="87"/>
-      <c r="G25" s="87" t="s">
+      <c r="D25" s="99"/>
+      <c r="E25" s="99"/>
+      <c r="F25" s="99"/>
+      <c r="G25" s="99" t="s">
         <v>99</v>
       </c>
-      <c r="H25" s="90"/>
+      <c r="H25" s="100"/>
       <c r="I25" s="25"/>
       <c r="J25" s="25"/>
       <c r="K25" s="25"/>
@@ -5198,16 +5202,16 @@
     <row r="26" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="25"/>
       <c r="B26" s="2"/>
-      <c r="C26" s="86" t="s">
+      <c r="C26" s="96" t="s">
         <v>104</v>
       </c>
-      <c r="D26" s="86"/>
-      <c r="E26" s="86"/>
-      <c r="F26" s="86"/>
-      <c r="G26" s="118" t="s">
+      <c r="D26" s="96"/>
+      <c r="E26" s="96"/>
+      <c r="F26" s="96"/>
+      <c r="G26" s="86" t="s">
         <v>105</v>
       </c>
-      <c r="H26" s="119"/>
+      <c r="H26" s="101"/>
       <c r="I26" s="25"/>
       <c r="J26" s="25"/>
       <c r="K26" s="25"/>
@@ -5219,16 +5223,16 @@
     <row r="27" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="25"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="87" t="s">
+      <c r="C27" s="99" t="s">
         <v>97</v>
       </c>
-      <c r="D27" s="87"/>
-      <c r="E27" s="87"/>
-      <c r="F27" s="87"/>
-      <c r="G27" s="138" t="s">
+      <c r="D27" s="99"/>
+      <c r="E27" s="99"/>
+      <c r="F27" s="99"/>
+      <c r="G27" s="102" t="s">
         <v>98</v>
       </c>
-      <c r="H27" s="139"/>
+      <c r="H27" s="103"/>
       <c r="I27" s="25"/>
       <c r="J27" s="25"/>
       <c r="K27" s="25"/>
@@ -5240,16 +5244,16 @@
     <row r="28" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="29"/>
       <c r="B28" s="2"/>
-      <c r="C28" s="86" t="s">
+      <c r="C28" s="96" t="s">
         <v>54</v>
       </c>
-      <c r="D28" s="86"/>
-      <c r="E28" s="86"/>
-      <c r="F28" s="86"/>
-      <c r="G28" s="118" t="s">
-        <v>112</v>
-      </c>
-      <c r="H28" s="119"/>
+      <c r="D28" s="96"/>
+      <c r="E28" s="96"/>
+      <c r="F28" s="96"/>
+      <c r="G28" s="86" t="s">
+        <v>111</v>
+      </c>
+      <c r="H28" s="101"/>
       <c r="I28" s="27"/>
       <c r="J28" s="27"/>
       <c r="K28" s="27"/>
@@ -5261,16 +5265,16 @@
     <row r="29" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="29"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="87" t="s">
+      <c r="C29" s="99" t="s">
         <v>55</v>
       </c>
-      <c r="D29" s="87"/>
-      <c r="E29" s="87"/>
-      <c r="F29" s="87"/>
-      <c r="G29" s="150" t="s">
+      <c r="D29" s="99"/>
+      <c r="E29" s="99"/>
+      <c r="F29" s="99"/>
+      <c r="G29" s="122" t="s">
         <v>56</v>
       </c>
-      <c r="H29" s="90"/>
+      <c r="H29" s="100"/>
       <c r="I29" s="27"/>
       <c r="J29" s="27"/>
       <c r="K29" s="27"/>
@@ -5282,16 +5286,16 @@
     <row r="30" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="29"/>
       <c r="B30" s="2"/>
-      <c r="C30" s="86" t="s">
+      <c r="C30" s="96" t="s">
         <v>58</v>
       </c>
-      <c r="D30" s="86"/>
-      <c r="E30" s="86"/>
-      <c r="F30" s="86"/>
-      <c r="G30" s="129" t="s">
+      <c r="D30" s="96"/>
+      <c r="E30" s="96"/>
+      <c r="F30" s="96"/>
+      <c r="G30" s="123" t="s">
         <v>59</v>
       </c>
-      <c r="H30" s="130"/>
+      <c r="H30" s="124"/>
       <c r="I30" s="27"/>
       <c r="J30" s="27"/>
       <c r="K30" s="27"/>
@@ -5303,14 +5307,14 @@
     <row r="31" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="29"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="87" t="s">
+      <c r="C31" s="99" t="s">
         <v>60</v>
       </c>
-      <c r="D31" s="87"/>
-      <c r="E31" s="87"/>
-      <c r="F31" s="87"/>
-      <c r="G31" s="146"/>
-      <c r="H31" s="147"/>
+      <c r="D31" s="99"/>
+      <c r="E31" s="99"/>
+      <c r="F31" s="99"/>
+      <c r="G31" s="118"/>
+      <c r="H31" s="119"/>
       <c r="I31" s="27"/>
       <c r="J31" s="27"/>
       <c r="K31" s="27"/>
@@ -5322,14 +5326,14 @@
     <row r="32" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="29"/>
       <c r="B32" s="2"/>
-      <c r="C32" s="86" t="s">
+      <c r="C32" s="96" t="s">
         <v>62</v>
       </c>
-      <c r="D32" s="86"/>
-      <c r="E32" s="86"/>
-      <c r="F32" s="86"/>
-      <c r="G32" s="148"/>
-      <c r="H32" s="149"/>
+      <c r="D32" s="96"/>
+      <c r="E32" s="96"/>
+      <c r="F32" s="96"/>
+      <c r="G32" s="120"/>
+      <c r="H32" s="121"/>
       <c r="I32" s="27"/>
       <c r="J32" s="27"/>
       <c r="K32" s="27"/>
@@ -5341,14 +5345,14 @@
     <row r="33" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="25"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="87" t="s">
+      <c r="C33" s="99" t="s">
         <v>102</v>
       </c>
-      <c r="D33" s="87"/>
-      <c r="E33" s="87"/>
-      <c r="F33" s="87"/>
-      <c r="G33" s="138"/>
-      <c r="H33" s="139"/>
+      <c r="D33" s="99"/>
+      <c r="E33" s="99"/>
+      <c r="F33" s="99"/>
+      <c r="G33" s="102"/>
+      <c r="H33" s="103"/>
       <c r="I33" s="27"/>
       <c r="J33" s="27"/>
       <c r="K33" s="27"/>
@@ -5359,15 +5363,15 @@
     </row>
     <row r="34" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="29"/>
-      <c r="B34" s="92" t="s">
+      <c r="B34" s="115" t="s">
         <v>93</v>
       </c>
-      <c r="C34" s="93"/>
-      <c r="D34" s="93"/>
-      <c r="E34" s="93"/>
-      <c r="F34" s="93"/>
-      <c r="G34" s="93"/>
-      <c r="H34" s="94"/>
+      <c r="C34" s="116"/>
+      <c r="D34" s="116"/>
+      <c r="E34" s="116"/>
+      <c r="F34" s="116"/>
+      <c r="G34" s="116"/>
+      <c r="H34" s="117"/>
       <c r="I34" s="27"/>
       <c r="J34" s="27"/>
       <c r="K34" s="27"/>
@@ -5378,11 +5382,11 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B35" s="65"/>
-      <c r="C35" s="131" t="s">
+      <c r="C35" s="125" t="s">
         <v>4</v>
       </c>
-      <c r="D35" s="132"/>
-      <c r="E35" s="133"/>
+      <c r="D35" s="126"/>
+      <c r="E35" s="127"/>
       <c r="F35" s="66" t="s">
         <v>5</v>
       </c>
@@ -5399,11 +5403,11 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B36" s="36"/>
-      <c r="C36" s="134" t="s">
+      <c r="C36" s="128" t="s">
         <v>0</v>
       </c>
-      <c r="D36" s="134"/>
-      <c r="E36" s="134"/>
+      <c r="D36" s="128"/>
+      <c r="E36" s="128"/>
       <c r="F36" s="37" t="s">
         <v>15</v>
       </c>
@@ -5421,11 +5425,11 @@
     <row r="37" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="29"/>
       <c r="B37" s="1"/>
-      <c r="C37" s="85" t="s">
-        <v>139</v>
-      </c>
-      <c r="D37" s="85"/>
-      <c r="E37" s="85"/>
+      <c r="C37" s="131" t="s">
+        <v>138</v>
+      </c>
+      <c r="D37" s="131"/>
+      <c r="E37" s="131"/>
       <c r="F37" s="69" t="s">
         <v>23</v>
       </c>
@@ -5446,19 +5450,19 @@
     <row r="38" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="29"/>
       <c r="B38" s="8"/>
-      <c r="C38" s="135" t="s">
+      <c r="C38" s="110" t="s">
+        <v>112</v>
+      </c>
+      <c r="D38" s="111"/>
+      <c r="E38" s="112"/>
+      <c r="F38" s="19" t="s">
         <v>113</v>
-      </c>
-      <c r="D38" s="136"/>
-      <c r="E38" s="137"/>
-      <c r="F38" s="19" t="s">
-        <v>114</v>
       </c>
       <c r="G38" s="17" t="s">
         <v>10</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I38" s="7"/>
       <c r="J38" s="29"/>
@@ -5470,19 +5474,19 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B39" s="1"/>
-      <c r="C39" s="85" t="s">
+      <c r="C39" s="131" t="s">
+        <v>139</v>
+      </c>
+      <c r="D39" s="131"/>
+      <c r="E39" s="131"/>
+      <c r="F39" s="28" t="s">
         <v>140</v>
-      </c>
-      <c r="D39" s="85"/>
-      <c r="E39" s="85"/>
-      <c r="F39" s="28" t="s">
-        <v>141</v>
       </c>
       <c r="G39" s="28" t="s">
         <v>24</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I39" s="27"/>
       <c r="J39" s="27"/>
@@ -5491,13 +5495,13 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B40" s="3"/>
-      <c r="C40" s="116" t="s">
+      <c r="C40" s="113" t="s">
         <v>21</v>
       </c>
-      <c r="D40" s="116"/>
-      <c r="E40" s="116"/>
+      <c r="D40" s="113"/>
+      <c r="E40" s="113"/>
       <c r="F40" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G40" s="17" t="s">
         <v>10</v>
@@ -5512,19 +5516,19 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B41" s="5"/>
-      <c r="C41" s="117" t="s">
+      <c r="C41" s="114" t="s">
         <v>26</v>
       </c>
-      <c r="D41" s="117"/>
-      <c r="E41" s="117"/>
+      <c r="D41" s="114"/>
+      <c r="E41" s="114"/>
       <c r="F41" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G41" s="28" t="s">
         <v>24</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I41" s="27"/>
       <c r="J41" s="27"/>
@@ -5533,19 +5537,19 @@
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B42" s="3"/>
-      <c r="C42" s="116" t="s">
+      <c r="C42" s="113" t="s">
         <v>27</v>
       </c>
-      <c r="D42" s="116"/>
-      <c r="E42" s="116"/>
+      <c r="D42" s="113"/>
+      <c r="E42" s="113"/>
       <c r="F42" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G42" s="17" t="s">
         <v>10</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I42" s="7"/>
       <c r="J42" s="27"/>
@@ -5554,19 +5558,19 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B43" s="5"/>
-      <c r="C43" s="117" t="s">
+      <c r="C43" s="114" t="s">
         <v>28</v>
       </c>
-      <c r="D43" s="117"/>
-      <c r="E43" s="117"/>
+      <c r="D43" s="114"/>
+      <c r="E43" s="114"/>
       <c r="F43" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G43" s="28" t="s">
         <v>24</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I43" s="7"/>
       <c r="J43" s="27"/>
@@ -5575,19 +5579,19 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B44" s="3"/>
-      <c r="C44" s="116" t="s">
+      <c r="C44" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="D44" s="116"/>
-      <c r="E44" s="116"/>
+      <c r="D44" s="113"/>
+      <c r="E44" s="113"/>
       <c r="F44" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G44" s="17" t="s">
         <v>10</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I44" s="7"/>
       <c r="J44" s="27"/>
@@ -5596,121 +5600,121 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B45" s="5"/>
-      <c r="C45" s="117" t="s">
+      <c r="C45" s="114" t="s">
         <v>30</v>
       </c>
-      <c r="D45" s="117"/>
-      <c r="E45" s="117"/>
+      <c r="D45" s="114"/>
+      <c r="E45" s="114"/>
       <c r="F45" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G45" s="28" t="s">
         <v>24</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I45" s="7"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B46" s="3"/>
-      <c r="C46" s="116" t="s">
+      <c r="C46" s="113" t="s">
         <v>31</v>
       </c>
-      <c r="D46" s="116"/>
-      <c r="E46" s="116"/>
+      <c r="D46" s="113"/>
+      <c r="E46" s="113"/>
       <c r="F46" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G46" s="17" t="s">
         <v>10</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I46" s="7"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B47" s="5"/>
-      <c r="C47" s="117" t="s">
+      <c r="C47" s="114" t="s">
         <v>32</v>
       </c>
-      <c r="D47" s="117"/>
-      <c r="E47" s="117"/>
+      <c r="D47" s="114"/>
+      <c r="E47" s="114"/>
       <c r="F47" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G47" s="28" t="s">
         <v>24</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I47" s="7"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B48" s="3"/>
-      <c r="C48" s="116" t="s">
+      <c r="C48" s="113" t="s">
         <v>33</v>
       </c>
-      <c r="D48" s="116"/>
-      <c r="E48" s="116"/>
+      <c r="D48" s="113"/>
+      <c r="E48" s="113"/>
       <c r="F48" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G48" s="17" t="s">
         <v>10</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I48" s="7"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B49" s="5"/>
-      <c r="C49" s="117" t="s">
+      <c r="C49" s="114" t="s">
         <v>34</v>
       </c>
-      <c r="D49" s="117"/>
-      <c r="E49" s="117"/>
+      <c r="D49" s="114"/>
+      <c r="E49" s="114"/>
       <c r="F49" s="18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G49" s="28" t="s">
         <v>24</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I49" s="7"/>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B50" s="3"/>
-      <c r="C50" s="116" t="s">
+      <c r="C50" s="113" t="s">
         <v>35</v>
       </c>
-      <c r="D50" s="116"/>
-      <c r="E50" s="116"/>
+      <c r="D50" s="113"/>
+      <c r="E50" s="113"/>
       <c r="F50" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G50" s="17" t="s">
         <v>10</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I50" s="7"/>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B51" s="5"/>
-      <c r="C51" s="117" t="s">
+      <c r="C51" s="114" t="s">
         <v>36</v>
       </c>
-      <c r="D51" s="117"/>
-      <c r="E51" s="117"/>
+      <c r="D51" s="114"/>
+      <c r="E51" s="114"/>
       <c r="F51" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G51" s="28" t="s">
         <v>24</v>
@@ -5723,19 +5727,19 @@
     <row r="52" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="29"/>
       <c r="B52" s="1"/>
-      <c r="C52" s="85" t="s">
+      <c r="C52" s="131" t="s">
+        <v>141</v>
+      </c>
+      <c r="D52" s="131"/>
+      <c r="E52" s="131"/>
+      <c r="F52" s="69" t="s">
         <v>142</v>
-      </c>
-      <c r="D52" s="85"/>
-      <c r="E52" s="85"/>
-      <c r="F52" s="69" t="s">
-        <v>143</v>
       </c>
       <c r="G52" s="69" t="s">
         <v>24</v>
       </c>
       <c r="H52" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I52" s="68"/>
       <c r="J52" s="68"/>
@@ -5748,11 +5752,11 @@
     <row r="53" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="14"/>
       <c r="B53" s="8"/>
-      <c r="C53" s="135" t="s">
+      <c r="C53" s="110" t="s">
         <v>38</v>
       </c>
-      <c r="D53" s="136"/>
-      <c r="E53" s="137"/>
+      <c r="D53" s="111"/>
+      <c r="E53" s="112"/>
       <c r="F53" s="19" t="s">
         <v>22</v>
       </c>
@@ -5760,7 +5764,7 @@
         <v>10</v>
       </c>
       <c r="H53" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I53" s="7"/>
       <c r="J53" s="14"/>
@@ -5773,13 +5777,13 @@
     <row r="54" spans="1:15" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="14"/>
       <c r="B54" s="9"/>
-      <c r="C54" s="143" t="s">
+      <c r="C54" s="107" t="s">
         <v>10</v>
       </c>
-      <c r="D54" s="144"/>
-      <c r="E54" s="145"/>
+      <c r="D54" s="108"/>
+      <c r="E54" s="109"/>
       <c r="F54" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G54" s="20" t="s">
         <v>11</v>
@@ -5797,11 +5801,11 @@
     </row>
     <row r="55" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="3"/>
-      <c r="C55" s="140" t="s">
+      <c r="C55" s="104" t="s">
         <v>95</v>
       </c>
-      <c r="D55" s="141"/>
-      <c r="E55" s="142"/>
+      <c r="D55" s="105"/>
+      <c r="E55" s="106"/>
       <c r="F55" s="17" t="s">
         <v>96</v>
       </c>
@@ -5812,45 +5816,45 @@
       <c r="I55" s="7"/>
     </row>
     <row r="56" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="120" t="s">
-        <v>145</v>
-      </c>
-      <c r="C56" s="121"/>
-      <c r="D56" s="121"/>
-      <c r="E56" s="121"/>
-      <c r="F56" s="121"/>
-      <c r="G56" s="121"/>
-      <c r="H56" s="122"/>
+      <c r="B56" s="132" t="s">
+        <v>144</v>
+      </c>
+      <c r="C56" s="133"/>
+      <c r="D56" s="133"/>
+      <c r="E56" s="133"/>
+      <c r="F56" s="133"/>
+      <c r="G56" s="133"/>
+      <c r="H56" s="134"/>
       <c r="I56" s="24"/>
     </row>
     <row r="57" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="123"/>
-      <c r="C57" s="124"/>
-      <c r="D57" s="124"/>
-      <c r="E57" s="124"/>
-      <c r="F57" s="124"/>
-      <c r="G57" s="124"/>
-      <c r="H57" s="125"/>
+      <c r="B57" s="135"/>
+      <c r="C57" s="136"/>
+      <c r="D57" s="136"/>
+      <c r="E57" s="136"/>
+      <c r="F57" s="136"/>
+      <c r="G57" s="136"/>
+      <c r="H57" s="137"/>
       <c r="I57" s="24"/>
     </row>
     <row r="58" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="123"/>
-      <c r="C58" s="124"/>
-      <c r="D58" s="124"/>
-      <c r="E58" s="124"/>
-      <c r="F58" s="124"/>
-      <c r="G58" s="124"/>
-      <c r="H58" s="125"/>
+      <c r="B58" s="135"/>
+      <c r="C58" s="136"/>
+      <c r="D58" s="136"/>
+      <c r="E58" s="136"/>
+      <c r="F58" s="136"/>
+      <c r="G58" s="136"/>
+      <c r="H58" s="137"/>
       <c r="I58" s="24"/>
     </row>
     <row r="59" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B59" s="126"/>
-      <c r="C59" s="127"/>
-      <c r="D59" s="127"/>
-      <c r="E59" s="127"/>
-      <c r="F59" s="127"/>
-      <c r="G59" s="127"/>
-      <c r="H59" s="128"/>
+      <c r="B59" s="138"/>
+      <c r="C59" s="139"/>
+      <c r="D59" s="139"/>
+      <c r="E59" s="139"/>
+      <c r="F59" s="139"/>
+      <c r="G59" s="139"/>
+      <c r="H59" s="140"/>
       <c r="I59" s="24"/>
     </row>
     <row r="60" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -5869,8 +5873,8 @@
       <c r="D61" s="26"/>
       <c r="E61" s="26"/>
       <c r="F61" s="26"/>
-      <c r="G61" s="100"/>
-      <c r="H61" s="100"/>
+      <c r="G61" s="130"/>
+      <c r="H61" s="130"/>
     </row>
     <row r="62" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="26"/>
@@ -5878,8 +5882,8 @@
       <c r="D62" s="26"/>
       <c r="E62" s="26"/>
       <c r="F62" s="26"/>
-      <c r="G62" s="100"/>
-      <c r="H62" s="100"/>
+      <c r="G62" s="130"/>
+      <c r="H62" s="130"/>
     </row>
     <row r="63" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="26"/>
@@ -5887,14 +5891,14 @@
       <c r="D63" s="26"/>
       <c r="E63" s="26"/>
       <c r="F63" s="26"/>
-      <c r="G63" s="100"/>
-      <c r="H63" s="100"/>
+      <c r="G63" s="130"/>
+      <c r="H63" s="130"/>
     </row>
     <row r="64" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="100"/>
-      <c r="C64" s="100"/>
-      <c r="D64" s="100"/>
-      <c r="E64" s="100"/>
+      <c r="B64" s="130"/>
+      <c r="C64" s="130"/>
+      <c r="D64" s="130"/>
+      <c r="E64" s="130"/>
       <c r="F64" s="26"/>
       <c r="G64" s="26"/>
       <c r="H64" s="26"/>
@@ -6015,9 +6019,9 @@
     </row>
     <row r="91" spans="2:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B91" s="26"/>
-      <c r="C91" s="98"/>
-      <c r="D91" s="98"/>
-      <c r="E91" s="98"/>
+      <c r="C91" s="129"/>
+      <c r="D91" s="129"/>
+      <c r="E91" s="129"/>
       <c r="F91" s="26"/>
       <c r="G91" s="26"/>
       <c r="H91" s="26"/>
@@ -8238,21 +8242,59 @@
     </row>
   </sheetData>
   <mergeCells count="84">
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B8:B18"/>
+    <mergeCell ref="G2:H5"/>
+    <mergeCell ref="G61:H63"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C91:E91"/>
+    <mergeCell ref="B64:E64"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="B56:H59"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C52:E52"/>
+    <mergeCell ref="C33:F33"/>
     <mergeCell ref="G26:H26"/>
     <mergeCell ref="G27:H27"/>
     <mergeCell ref="C55:E55"/>
@@ -8269,59 +8311,21 @@
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="C30:F30"/>
     <mergeCell ref="G30:H30"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C91:E91"/>
-    <mergeCell ref="B64:E64"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="B56:H59"/>
-    <mergeCell ref="G2:H5"/>
-    <mergeCell ref="G61:H63"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C13:H13"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B8:B18"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C52:E52"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C12:F12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G18:H18" location="'Stack-up'!A1" display="See " xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -9182,7 +9186,7 @@
   </sheetPr>
   <dimension ref="C2:X33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M35" sqref="M35"/>
     </sheetView>
   </sheetViews>
@@ -9206,9 +9210,9 @@
       <c r="G2" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="U2" s="161"/>
-      <c r="V2" s="161"/>
-      <c r="W2" s="161"/>
+      <c r="U2" s="172"/>
+      <c r="V2" s="172"/>
+      <c r="W2" s="172"/>
     </row>
     <row r="3" spans="3:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="49" t="s">
@@ -9230,10 +9234,10 @@
       <c r="I3" s="40"/>
       <c r="J3" s="40"/>
       <c r="K3" s="40"/>
-      <c r="U3" s="164"/>
-      <c r="V3" s="164"/>
-      <c r="W3" s="164"/>
-      <c r="X3" s="161"/>
+      <c r="U3" s="173"/>
+      <c r="V3" s="173"/>
+      <c r="W3" s="173"/>
+      <c r="X3" s="172"/>
     </row>
     <row r="4" spans="3:24" x14ac:dyDescent="0.25">
       <c r="C4" s="57"/>
@@ -9243,7 +9247,7 @@
       <c r="E4" s="59">
         <v>48</v>
       </c>
-      <c r="F4" s="162">
+      <c r="F4" s="166">
         <f>E4+E5</f>
         <v>96</v>
       </c>
@@ -9252,10 +9256,10 @@
       <c r="I4" s="40"/>
       <c r="J4" s="40"/>
       <c r="K4" s="40"/>
-      <c r="U4" s="164"/>
-      <c r="V4" s="164"/>
-      <c r="W4" s="164"/>
-      <c r="X4" s="161"/>
+      <c r="U4" s="173"/>
+      <c r="V4" s="173"/>
+      <c r="W4" s="173"/>
+      <c r="X4" s="172"/>
     </row>
     <row r="5" spans="3:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="61"/>
@@ -9265,7 +9269,7 @@
       <c r="E5" s="63">
         <v>48</v>
       </c>
-      <c r="F5" s="163"/>
+      <c r="F5" s="167"/>
       <c r="G5" s="64"/>
       <c r="H5" s="75"/>
       <c r="I5" s="40"/>
@@ -9277,10 +9281,10 @@
       <c r="S5" s="12">
         <v>25.4</v>
       </c>
-      <c r="U5" s="164"/>
-      <c r="V5" s="164"/>
-      <c r="W5" s="164"/>
-      <c r="X5" s="161"/>
+      <c r="U5" s="173"/>
+      <c r="V5" s="173"/>
+      <c r="W5" s="173"/>
+      <c r="X5" s="172"/>
     </row>
     <row r="6" spans="3:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="49" t="s">
@@ -9300,21 +9304,21 @@
       <c r="I6" s="70"/>
       <c r="J6" s="71"/>
       <c r="K6" s="41"/>
-      <c r="U6" s="164"/>
-      <c r="V6" s="164"/>
-      <c r="W6" s="164"/>
-      <c r="X6" s="161"/>
+      <c r="U6" s="173"/>
+      <c r="V6" s="173"/>
+      <c r="W6" s="173"/>
+      <c r="X6" s="172"/>
     </row>
     <row r="7" spans="3:24" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7" s="43"/>
       <c r="D7" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="E7" s="173">
+      <c r="E7" s="85">
         <v>127</v>
       </c>
-      <c r="F7" s="165"/>
-      <c r="G7" s="166"/>
+      <c r="F7" s="170"/>
+      <c r="G7" s="171"/>
       <c r="H7" s="77"/>
       <c r="I7" s="71"/>
       <c r="J7" s="71"/>
@@ -9342,7 +9346,7 @@
         <v>81</v>
       </c>
       <c r="H8" s="73" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I8" s="72"/>
       <c r="J8" s="71"/>
@@ -9363,7 +9367,7 @@
       <c r="E9" s="59">
         <v>71</v>
       </c>
-      <c r="F9" s="162">
+      <c r="F9" s="166">
         <f>E9+E10</f>
         <v>142</v>
       </c>
@@ -9388,7 +9392,7 @@
       <c r="E10" s="63">
         <v>71</v>
       </c>
-      <c r="F10" s="163"/>
+      <c r="F10" s="167"/>
       <c r="G10" s="64"/>
       <c r="H10" s="78"/>
       <c r="I10" s="72"/>
@@ -9433,7 +9437,7 @@
       <c r="D12" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="E12" s="173">
+      <c r="E12" s="85">
         <v>127</v>
       </c>
       <c r="F12" s="45"/>
@@ -9470,7 +9474,7 @@
       <c r="E14" s="59">
         <v>71</v>
       </c>
-      <c r="F14" s="162">
+      <c r="F14" s="166">
         <f>E14+E15</f>
         <v>142</v>
       </c>
@@ -9488,7 +9492,7 @@
       <c r="E15" s="63">
         <v>71</v>
       </c>
-      <c r="F15" s="163"/>
+      <c r="F15" s="167"/>
       <c r="G15" s="64"/>
       <c r="H15" s="78"/>
       <c r="I15" s="72"/>
@@ -9510,7 +9514,7 @@
         <v>74</v>
       </c>
       <c r="H16" s="79" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I16" s="72"/>
       <c r="J16" s="71"/>
@@ -9521,7 +9525,7 @@
       <c r="D17" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="E17" s="173">
+      <c r="E17" s="85">
         <v>127</v>
       </c>
       <c r="F17" s="45"/>
@@ -9549,7 +9553,7 @@
         <v>81</v>
       </c>
       <c r="H18" s="73" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I18" s="72"/>
       <c r="J18" s="71"/>
@@ -9566,7 +9570,7 @@
       <c r="E19" s="59">
         <v>71</v>
       </c>
-      <c r="F19" s="162">
+      <c r="F19" s="166">
         <f>E19+E20</f>
         <v>142</v>
       </c>
@@ -9587,7 +9591,7 @@
       <c r="E20" s="63">
         <v>71</v>
       </c>
-      <c r="F20" s="163"/>
+      <c r="F20" s="167"/>
       <c r="G20" s="64"/>
       <c r="H20" s="75"/>
       <c r="I20" s="72"/>
@@ -9618,7 +9622,7 @@
       <c r="D22" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="E22" s="173">
+      <c r="E22" s="85">
         <v>127</v>
       </c>
       <c r="F22" s="45"/>
@@ -9655,7 +9659,7 @@
       <c r="E24" s="59">
         <v>71</v>
       </c>
-      <c r="F24" s="162">
+      <c r="F24" s="166">
         <f>E24+E25</f>
         <v>142</v>
       </c>
@@ -9673,7 +9677,7 @@
       <c r="E25" s="63">
         <v>71</v>
       </c>
-      <c r="F25" s="163"/>
+      <c r="F25" s="167"/>
       <c r="G25" s="64"/>
       <c r="H25" s="78"/>
       <c r="I25" s="72"/>
@@ -9695,7 +9699,7 @@
         <v>74</v>
       </c>
       <c r="H26" s="79" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I26" s="72"/>
       <c r="J26" s="71"/>
@@ -9706,11 +9710,11 @@
       <c r="D27" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="E27" s="173">
+      <c r="E27" s="85">
         <v>127</v>
       </c>
-      <c r="F27" s="171"/>
-      <c r="G27" s="172"/>
+      <c r="F27" s="168"/>
+      <c r="G27" s="169"/>
       <c r="H27" s="77"/>
       <c r="I27" s="72"/>
       <c r="J27" s="71"/>
@@ -9743,7 +9747,7 @@
       <c r="E29" s="59">
         <v>48</v>
       </c>
-      <c r="F29" s="162">
+      <c r="F29" s="166">
         <f>E29+E30</f>
         <v>96</v>
       </c>
@@ -9761,7 +9765,7 @@
       <c r="E30" s="63">
         <v>48</v>
       </c>
-      <c r="F30" s="163"/>
+      <c r="F30" s="167"/>
       <c r="G30" s="64"/>
       <c r="H30" s="75"/>
       <c r="I30" s="40"/>
@@ -9801,15 +9805,15 @@
       <c r="K32" s="47"/>
     </row>
     <row r="33" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="169" t="s">
+      <c r="C33" s="164" t="s">
         <v>88</v>
       </c>
-      <c r="D33" s="170"/>
-      <c r="E33" s="167">
+      <c r="D33" s="165"/>
+      <c r="E33" s="162">
         <f>SUM(E3:E31)</f>
         <v>2023</v>
       </c>
-      <c r="F33" s="168"/>
+      <c r="F33" s="163"/>
       <c r="G33" s="34"/>
       <c r="H33" s="84"/>
       <c r="I33" s="70"/>
@@ -9818,13 +9822,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="F14:F15"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F29:F30"/>
     <mergeCell ref="U2:W2"/>
@@ -9833,6 +9830,13 @@
     <mergeCell ref="U5:W6"/>
     <mergeCell ref="X5:X6"/>
     <mergeCell ref="U3:W4"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="F14:F15"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="46" orientation="landscape" r:id="rId1"/>

</xml_diff>